<commit_message>
add real feature engineering v0.2
</commit_message>
<xml_diff>
--- a/supermarket/prj/feature/feature_list_v1.2.xlsx
+++ b/supermarket/prj/feature/feature_list_v1.2.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03_SoftwareDev\00_MachineLearning\08_repo\CCF\MachineLearning_Matches\supermarket\prj\feature\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101">
   <si>
     <t>基础特征</t>
   </si>
@@ -43,6 +38,9 @@
   </si>
   <si>
     <t>节日:3,假日：2，工作日：1</t>
+  </si>
+  <si>
+    <t>disHoliday</t>
   </si>
   <si>
     <t>假日（20150101，20150218,20150404,20150501为距离起点）距离权值: 
@@ -232,6 +230,9 @@
     <t>price_median</t>
   </si>
   <si>
+    <t>类别价格中位数                                           [需在原始表计算]</t>
+  </si>
+  <si>
     <t>bonusRatio</t>
   </si>
   <si>
@@ -395,21 +396,19 @@
   </si>
   <si>
     <t>当日起过去一天(1th， -7)与过去21天(15th，-21)的销量差值，diff14</t>
-  </si>
-  <si>
-    <t>类别价格中位数                                           [需在原始表计算]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>disHoliday</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,32 +418,356 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -452,14 +775,256 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -468,23 +1033,68 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <i val="0"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFD7D7D7"/>
         </patternFill>
       </fill>
@@ -495,9 +1105,7 @@
         <i val="0"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
+        <patternFill patternType="none"/>
       </fill>
     </dxf>
   </dxfs>
@@ -510,9 +1118,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -799,19 +1404,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="3" max="3" width="28.125" customWidth="1"/>
@@ -819,8 +1424,8 @@
     <col min="7" max="7" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -833,8 +1438,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -845,8 +1450,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -859,553 +1464,553 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1">
+    <row r="5" ht="94.5" spans="1:4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4"/>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4"/>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4"/>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="81" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1">
+    </row>
+    <row r="10" ht="81" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="4"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1"/>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="4"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="4"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1"/>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="4"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1"/>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1"/>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="4"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1"/>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1"/>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="4"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1"/>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="4"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1"/>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="4"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1"/>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="4"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1"/>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="4"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1"/>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="4"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1"/>
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1"/>
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="4"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1"/>
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="4"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1"/>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="4"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1"/>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="4"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1"/>
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="4"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1"/>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="4"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1"/>
       <c r="B36">
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="4"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1"/>
       <c r="B37">
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="4"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1"/>
       <c r="B38">
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="4"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1"/>
       <c r="B39">
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="4"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1"/>
       <c r="B40">
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="4"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1"/>
       <c r="B41">
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A42" s="4"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" ht="40.5" spans="1:4">
+      <c r="A42" s="1"/>
       <c r="B42">
         <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A43" s="4"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" ht="40.5" spans="1:4">
+      <c r="A43" s="1"/>
       <c r="B43">
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A44" s="4"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" ht="40.5" spans="1:4">
+      <c r="A44" s="1"/>
       <c r="B44">
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="4"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1"/>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="4"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1"/>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="4"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1"/>
       <c r="B47">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="4"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1"/>
       <c r="B48">
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="4"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1"/>
       <c r="B49">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3">
       <c r="C50" s="2"/>
     </row>
   </sheetData>
@@ -1416,8 +2021,8 @@
     <mergeCell ref="A10:A28"/>
     <mergeCell ref="A29:A49"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add rolling price feature
</commit_message>
<xml_diff>
--- a/supermarket/prj/feature/feature_list_v1.2.xlsx
+++ b/supermarket/prj/feature/feature_list_v1.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,10 +403,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -414,13 +414,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -440,23 +433,22 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -477,6 +469,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -485,44 +515,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -539,20 +531,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,6 +539,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -582,187 +582,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -786,21 +786,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -830,6 +815,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -847,9 +841,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -862,27 +873,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -891,133 +891,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1412,8 +1412,8 @@
   <sheetPr/>
   <dimension ref="A2:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
add all features v1.0
</commit_message>
<xml_diff>
--- a/supermarket/prj/feature/feature_list_v1.2.xlsx
+++ b/supermarket/prj/feature/feature_list_v1.2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_SoftwareDev\05_MachineLearning\00_Match\03_CCF\MachineLearning_Matches\supermarket\prj\feature\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28692" windowHeight="13056"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>基础特征</t>
   </si>
@@ -344,9 +349,6 @@
     <t>商品当日起过去一月销量中位数，若为NA则为当日销量</t>
   </si>
   <si>
-    <t>weekOn1WeekRatio</t>
-  </si>
-  <si>
     <t>当日起过去一周与过去两周销量比值，同比
 例：上周二与上上周二的销量比值
 NA为1</t>
@@ -368,196 +370,53 @@
 NA为1</t>
   </si>
   <si>
-    <t>day3OverWeek3TotRatio</t>
+    <t>当日起过去七天(1th， -7)与过去八天(2th，-8)的销量差值，diff1</t>
+  </si>
+  <si>
+    <t>dayOn2DayDiff</t>
+  </si>
+  <si>
+    <t>当日起过去一天(1th， -7)与过去九天(3th，-9)的销量差值，diff2</t>
+  </si>
+  <si>
+    <t>dayOn7DayDiff</t>
+  </si>
+  <si>
+    <t>当日起过去一天(1th， -7)与过去14天(8th，-14)的销量差值，diff7</t>
+  </si>
+  <si>
+    <t>dayOn14DayDiff</t>
+  </si>
+  <si>
+    <t>当日起过去一天(1th， -7)与过去21天(15th，-21)的销量差值，diff14</t>
+  </si>
+  <si>
+    <t>weekOn1WeekRatio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>当日起过去一周七天与过去三周总量的比值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>day3OoverWeek3TotRatio</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>dayOn1DayDiff</t>
-  </si>
-  <si>
-    <t>当日起过去七天(1th， -7)与过去八天(2th，-8)的销量差值，diff1</t>
-  </si>
-  <si>
-    <t>dayOn2DayDiff</t>
-  </si>
-  <si>
-    <t>当日起过去一天(1th， -7)与过去九天(3th，-9)的销量差值，diff2</t>
-  </si>
-  <si>
-    <t>dayOn7DayDiff</t>
-  </si>
-  <si>
-    <t>当日起过去一天(1th， -7)与过去14天(8th，-14)的销量差值，diff7</t>
-  </si>
-  <si>
-    <t>dayOn14DayDiff</t>
-  </si>
-  <si>
-    <t>当日起过去一天(1th， -7)与过去21天(15th，-21)的销量差值，diff14</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -572,202 +431,22 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -775,257 +454,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1033,64 +467,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
       </font>
       <fill>
@@ -1118,6 +507,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1404,28 +796,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="3" max="3" width="28.125" customWidth="1"/>
-    <col min="4" max="4" width="92.75" customWidth="1"/>
-    <col min="7" max="7" width="8.875" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="4" width="92.77734375" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -1438,8 +830,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -1450,8 +842,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -1464,19 +856,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="94.5" spans="1:4">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2">
+    <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1490,7 +882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7">
         <v>6</v>
@@ -1502,7 +894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8">
         <v>7</v>
@@ -1514,7 +906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9">
         <v>8</v>
@@ -1526,22 +918,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" ht="81" spans="1:4">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11">
         <v>10</v>
       </c>
@@ -1552,8 +944,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
       <c r="B12">
         <v>11</v>
       </c>
@@ -1564,8 +956,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
       <c r="B13">
         <v>12</v>
       </c>
@@ -1576,8 +968,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
       <c r="B14">
         <v>13</v>
       </c>
@@ -1588,8 +980,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
       <c r="B15">
         <v>14</v>
       </c>
@@ -1600,8 +992,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
       <c r="B16">
         <v>15</v>
       </c>
@@ -1612,8 +1004,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
       <c r="B17">
         <v>16</v>
       </c>
@@ -1624,8 +1016,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
       <c r="B18">
         <v>17</v>
       </c>
@@ -1636,8 +1028,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
       <c r="B19">
         <v>18</v>
       </c>
@@ -1648,8 +1040,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
       <c r="B20">
         <v>19</v>
       </c>
@@ -1660,8 +1052,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
       <c r="B21">
         <v>20</v>
       </c>
@@ -1672,8 +1064,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
       <c r="B22">
         <v>21</v>
       </c>
@@ -1684,8 +1076,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
       <c r="B23">
         <v>22</v>
       </c>
@@ -1696,8 +1088,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
       <c r="B24">
         <v>23</v>
       </c>
@@ -1708,8 +1100,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
       <c r="B25">
         <v>24</v>
       </c>
@@ -1720,8 +1112,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
       <c r="B26">
         <v>25</v>
       </c>
@@ -1732,8 +1124,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
       <c r="B27">
         <v>26</v>
       </c>
@@ -1744,8 +1136,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
       <c r="B28">
         <v>27</v>
       </c>
@@ -1756,8 +1148,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B29">
@@ -1770,8 +1162,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
       <c r="B30">
         <v>29</v>
       </c>
@@ -1782,8 +1174,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
       <c r="B31">
         <v>30</v>
       </c>
@@ -1794,8 +1186,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
       <c r="B32">
         <v>31</v>
       </c>
@@ -1806,8 +1198,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
       <c r="B33">
         <v>32</v>
       </c>
@@ -1818,8 +1210,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1"/>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
       <c r="B34">
         <v>33</v>
       </c>
@@ -1830,8 +1222,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
       <c r="B35">
         <v>34</v>
       </c>
@@ -1842,8 +1234,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
       <c r="B36">
         <v>35</v>
       </c>
@@ -1854,8 +1246,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
       <c r="B37">
         <v>36</v>
       </c>
@@ -1866,8 +1258,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
       <c r="B38">
         <v>37</v>
       </c>
@@ -1878,8 +1270,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
       <c r="B39">
         <v>38</v>
       </c>
@@ -1890,8 +1282,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
       <c r="B40">
         <v>39</v>
       </c>
@@ -1902,8 +1294,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1"/>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
       <c r="B41">
         <v>40</v>
       </c>
@@ -1914,104 +1306,104 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" ht="40.5" spans="1:4">
-      <c r="A42" s="1"/>
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
       <c r="B42">
         <v>41</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" ht="40.5" spans="1:4">
-      <c r="A43" s="1"/>
+    </row>
+    <row r="43" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
       <c r="B43">
         <v>42</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" ht="40.5" spans="1:4">
-      <c r="A44" s="1"/>
+    </row>
+    <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
       <c r="B44">
         <v>43</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
       <c r="B45">
         <v>44</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
       <c r="B46">
         <v>45</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
       <c r="B47">
         <v>46</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
       <c r="B48">
         <v>47</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
       <c r="B49">
         <v>48</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" s="2"/>
+      <c r="C49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2021,8 +1413,8 @@
     <mergeCell ref="A10:A28"/>
     <mergeCell ref="A29:A49"/>
   </mergeCells>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>